<commit_message>
Muitas alterações feitas em conjunto, Projeto quase final
</commit_message>
<xml_diff>
--- a/Avaliação Experimental.xlsx
+++ b/Avaliação Experimental.xlsx
@@ -272,11 +272,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2101010480"/>
-        <c:axId val="-2104453152"/>
+        <c:axId val="-2132889104"/>
+        <c:axId val="-2132882192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2101010480"/>
+        <c:axId val="-2132889104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,8 +356,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -380,12 +381,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2104453152"/>
+        <c:crossAx val="-2132882192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2104453152"/>
+        <c:axId val="-2132882192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -494,7 +495,487 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101010480"/>
+        <c:crossAx val="-2132889104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT" sz="1800"/>
+              <a:t>Tempo de execução em função do número de vértices e arestas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.130595059205386"/>
+          <c:y val="0.048695652173913"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$B$23:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>58783.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117566.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>235132.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>470264.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>940528.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.881056E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.762112E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$C$23:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.192</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.342</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.659</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.343</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2089661408"/>
+        <c:axId val="-2089698896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2089661408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Número de vértices + arestas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2089698896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2089698896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT" sz="1400"/>
+                  <a:t>Tempo de execução (segundos)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2089661408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -586,7 +1067,585 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1151,6 +2210,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1422,13 +2513,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2">
@@ -1484,6 +2578,68 @@
         <v>0.24299999999999999</v>
       </c>
     </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>58783</v>
+      </c>
+      <c r="C23">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f>B23*2</f>
+        <v>117566</v>
+      </c>
+      <c r="C24">
+        <v>8.6999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <f t="shared" ref="B25:B29" si="0">B24*2</f>
+        <v>235132</v>
+      </c>
+      <c r="C25">
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>470264</v>
+      </c>
+      <c r="C26">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>940528</v>
+      </c>
+      <c r="C27">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1881056</v>
+      </c>
+      <c r="C28">
+        <v>1.343</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>3762112</v>
+      </c>
+      <c r="C29">
+        <v>2.7149999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>